<commit_message>
IDwr and IDov update
 - re-downloaded data
</commit_message>
<xml_diff>
--- a/Idaho/Overlays/IDov_Overlay Schema Mapping to WaDE.xlsx
+++ b/Idaho/Overlays/IDov_Overlay Schema Mapping to WaDE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Idaho\Overlays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DB067A-5EDA-4BA5-8F96-3080C693E2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF0B938-E386-4E9C-B838-D218B8600511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="645" firstSheet="1" activeTab="1" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="645" firstSheet="1" activeTab="3" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -1819,7 +1819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203F7812-755D-4EFC-B094-8BF895453DC0}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>